<commit_message>
refactor: changing code structure
Graphs are working using a for loop with .append()
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -7,21 +7,21 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="47" sheetId="1" r:id="rId1"/>
-    <sheet name="52" sheetId="2" r:id="rId2"/>
-    <sheet name="57" sheetId="3" r:id="rId3"/>
-    <sheet name="63" sheetId="4" r:id="rId4"/>
-    <sheet name="69" sheetId="5" r:id="rId5"/>
-    <sheet name="76" sheetId="6" r:id="rId6"/>
-    <sheet name="84" sheetId="7" r:id="rId7"/>
-    <sheet name="84+" sheetId="8" r:id="rId8"/>
+    <sheet name="59" sheetId="1" r:id="rId1"/>
+    <sheet name="66" sheetId="2" r:id="rId2"/>
+    <sheet name="74" sheetId="3" r:id="rId3"/>
+    <sheet name="83" sheetId="4" r:id="rId4"/>
+    <sheet name="93" sheetId="5" r:id="rId5"/>
+    <sheet name="105" sheetId="6" r:id="rId6"/>
+    <sheet name="120" sheetId="7" r:id="rId7"/>
+    <sheet name="120+" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="71">
   <si>
     <t>Name</t>
   </si>
@@ -29,205 +29,211 @@
     <t>Goodlift</t>
   </si>
   <si>
-    <t>Tiffany Chapon</t>
-  </si>
-  <si>
-    <t>Noémie Allabert</t>
-  </si>
-  <si>
-    <t>Stéphanie Legard</t>
-  </si>
-  <si>
-    <t>Andréa Zicaro</t>
-  </si>
-  <si>
-    <t>Bénédicte LePanse</t>
-  </si>
-  <si>
-    <t>Cathy Phatien</t>
-  </si>
-  <si>
-    <t>Nathalie Piantino</t>
-  </si>
-  <si>
-    <t>Marianne Bouvard</t>
-  </si>
-  <si>
-    <t>Yvelise Martin</t>
-  </si>
-  <si>
-    <t>Nathalie Feraud</t>
-  </si>
-  <si>
-    <t>Shizuka Rico</t>
-  </si>
-  <si>
-    <t>Camille Hadrys</t>
-  </si>
-  <si>
-    <t>Alison Huet</t>
-  </si>
-  <si>
-    <t>Laurie Julien</t>
-  </si>
-  <si>
-    <t>Anna Maramotti</t>
-  </si>
-  <si>
-    <t>Lorraine Balbiani</t>
-  </si>
-  <si>
-    <t>Maëva Lambert</t>
-  </si>
-  <si>
-    <t>Jade Jacob</t>
-  </si>
-  <si>
-    <t>Océane Regis</t>
-  </si>
-  <si>
-    <t>Sovannphaktra Pal</t>
-  </si>
-  <si>
-    <t>Caroline Suné</t>
-  </si>
-  <si>
-    <t>Agnès Alves</t>
-  </si>
-  <si>
-    <t>Léa Gratacos</t>
-  </si>
-  <si>
-    <t>Mélodie Anthouard</t>
-  </si>
-  <si>
-    <t>Mélanie Pagesy</t>
-  </si>
-  <si>
-    <t>Marina Soyer-Bardi</t>
-  </si>
-  <si>
-    <t>Prescillia Bavoil</t>
-  </si>
-  <si>
-    <t>Samantha Eugenie</t>
-  </si>
-  <si>
-    <t>Ludivine Delos</t>
-  </si>
-  <si>
-    <t>Mathilde Rosset</t>
-  </si>
-  <si>
-    <t>Sarah Saint Aime</t>
-  </si>
-  <si>
-    <t>Justine Jouve</t>
-  </si>
-  <si>
-    <t>Mathilde Pataille</t>
-  </si>
-  <si>
-    <t>Clara Peyraud</t>
-  </si>
-  <si>
-    <t>Pauline Le Bras</t>
-  </si>
-  <si>
-    <t>Andorina Bouchoux</t>
-  </si>
-  <si>
-    <t>Bertille Hedon</t>
-  </si>
-  <si>
-    <t>Camille Pailha</t>
-  </si>
-  <si>
-    <t>Clara Kaminski</t>
-  </si>
-  <si>
-    <t>Haingotiana Rasamimanantsoa</t>
-  </si>
-  <si>
-    <t>Isoline Berger</t>
-  </si>
-  <si>
-    <t>Laura Mautalen</t>
-  </si>
-  <si>
-    <t>Margot Concolato</t>
-  </si>
-  <si>
-    <t>Angeline Berva</t>
-  </si>
-  <si>
-    <t>Christelle Mouandjo</t>
-  </si>
-  <si>
-    <t>Jessica Doorhyee</t>
-  </si>
-  <si>
-    <t>France Juilien</t>
-  </si>
-  <si>
-    <t>Pauline Leroux</t>
-  </si>
-  <si>
-    <t>Ludivine Leroy</t>
-  </si>
-  <si>
-    <t>Elisa Elleuch</t>
-  </si>
-  <si>
-    <t>Kelly Millecamps</t>
-  </si>
-  <si>
-    <t>Lea Schreiner</t>
-  </si>
-  <si>
-    <t>Innès Allouache</t>
-  </si>
-  <si>
-    <t>Marion Attelly</t>
-  </si>
-  <si>
-    <t>Julie Franch Guerra</t>
-  </si>
-  <si>
-    <t>Cécile Brotons</t>
-  </si>
-  <si>
-    <t>France Collinot</t>
-  </si>
-  <si>
-    <t>Amélie Mierger</t>
-  </si>
-  <si>
-    <t>Marie Stéphanie Vili</t>
-  </si>
-  <si>
-    <t>Rachelle Letaief</t>
-  </si>
-  <si>
-    <t>Atonina Vehikite</t>
-  </si>
-  <si>
-    <t>Cindy Hebe</t>
-  </si>
-  <si>
-    <t>Camille Dezier</t>
-  </si>
-  <si>
-    <t>Albane Benitah</t>
-  </si>
-  <si>
-    <t>Jennifer Bailleul</t>
-  </si>
-  <si>
-    <t>Camellia Messaoui</t>
-  </si>
-  <si>
-    <t>Angélique Lafont</t>
+    <t>Antoine Garcia</t>
+  </si>
+  <si>
+    <t>Etienne Lited</t>
+  </si>
+  <si>
+    <t>Thomas Acher</t>
+  </si>
+  <si>
+    <t>Julien Gutierrez</t>
+  </si>
+  <si>
+    <t>Hermann Charbonnier</t>
+  </si>
+  <si>
+    <t>Thibault Leparc</t>
+  </si>
+  <si>
+    <t>Vincent Todaro</t>
+  </si>
+  <si>
+    <t>Loïz Gautier</t>
+  </si>
+  <si>
+    <t>Gael Pannier</t>
+  </si>
+  <si>
+    <t>Adrien Mailler</t>
+  </si>
+  <si>
+    <t>Panagiotis Tarinidis</t>
+  </si>
+  <si>
+    <t>Hassan El Belghiti</t>
+  </si>
+  <si>
+    <t>Thomas Louet</t>
+  </si>
+  <si>
+    <t>Julien Mercier #2</t>
+  </si>
+  <si>
+    <t>Arthur Hauet</t>
+  </si>
+  <si>
+    <t>Valentin Fruchard</t>
+  </si>
+  <si>
+    <t>Maxime Bataillard</t>
+  </si>
+  <si>
+    <t>Alexandre Tarinidis</t>
+  </si>
+  <si>
+    <t>Steve Vigouroux</t>
+  </si>
+  <si>
+    <t>Paul Rembauville</t>
+  </si>
+  <si>
+    <t>Adrien Poinson</t>
+  </si>
+  <si>
+    <t>Andréa Bonetto</t>
+  </si>
+  <si>
+    <t>Bastien Poyet</t>
+  </si>
+  <si>
+    <t>Alexandre Pont</t>
+  </si>
+  <si>
+    <t>Khaled Benbachir</t>
+  </si>
+  <si>
+    <t>Charly Mairesse</t>
+  </si>
+  <si>
+    <t>Florian Magnier</t>
+  </si>
+  <si>
+    <t>Yanis Bouchou</t>
+  </si>
+  <si>
+    <t>Guillaume Parisot</t>
+  </si>
+  <si>
+    <t>Pierre Renaud</t>
+  </si>
+  <si>
+    <t>Valentin Cure</t>
+  </si>
+  <si>
+    <t>Souleiman Turki</t>
+  </si>
+  <si>
+    <t>Thomas Czaplicki</t>
+  </si>
+  <si>
+    <t>Romain Picot-Guéraud</t>
+  </si>
+  <si>
+    <t>Maxime Girard</t>
+  </si>
+  <si>
+    <t>Joris Quai</t>
+  </si>
+  <si>
+    <t>Anthony Costarigot</t>
+  </si>
+  <si>
+    <t>Richmond Baiden</t>
+  </si>
+  <si>
+    <t>Julien Balangwe Bakinien</t>
+  </si>
+  <si>
+    <t>Ali Ben Hadj Ali</t>
+  </si>
+  <si>
+    <t>Quentin Gilbert</t>
+  </si>
+  <si>
+    <t>Guillaume Jean Marie Flore</t>
+  </si>
+  <si>
+    <t>Malik Bernoussi Triolet</t>
+  </si>
+  <si>
+    <t>Paco Castillo</t>
+  </si>
+  <si>
+    <t>Gil Pinheiro</t>
+  </si>
+  <si>
+    <t>Gabriel Begue</t>
+  </si>
+  <si>
+    <t>Corentin Clément</t>
+  </si>
+  <si>
+    <t>Nicolas Peyraud</t>
+  </si>
+  <si>
+    <t>Sofiane Belkesir</t>
+  </si>
+  <si>
+    <t>Benoit Carole</t>
+  </si>
+  <si>
+    <t>Sami Maury</t>
+  </si>
+  <si>
+    <t>Rekendy Faufil</t>
+  </si>
+  <si>
+    <t>Youssuf El Adlani</t>
+  </si>
+  <si>
+    <t>Antoine De Rohden</t>
+  </si>
+  <si>
+    <t>Charly Boucher</t>
+  </si>
+  <si>
+    <t>Tony Bayrakcioglu</t>
+  </si>
+  <si>
+    <t>Frédéric Lecellier</t>
+  </si>
+  <si>
+    <t>Andy Richon</t>
+  </si>
+  <si>
+    <t>Nour-Eddine Ghaoui</t>
+  </si>
+  <si>
+    <t>Marcus Feliho</t>
+  </si>
+  <si>
+    <t>Romuald Massé</t>
+  </si>
+  <si>
+    <t>Stanley Odin</t>
+  </si>
+  <si>
+    <t>Julien Moala</t>
+  </si>
+  <si>
+    <t>Ugo Masarotti</t>
+  </si>
+  <si>
+    <t>Paulin Mbakop Kweffo</t>
+  </si>
+  <si>
+    <t>Abdellah Hassar</t>
+  </si>
+  <si>
+    <t>Karim Messai</t>
+  </si>
+  <si>
+    <t>Éric Bonin</t>
+  </si>
+  <si>
+    <t>Abdelaziz Benikken</t>
   </si>
 </sst>
 </file>
@@ -601,13 +607,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2">
-        <v>118.48</v>
+        <v>94.15000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -618,95 +624,95 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>104.62</v>
+        <v>93.94</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1">
-        <v>47</v>
+        <v>137</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4">
-        <v>101.62</v>
+        <v>90.45</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1">
-        <v>2</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5">
-        <v>92.38</v>
+        <v>89.2</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6">
-        <v>92</v>
+        <v>84.81999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>134</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7">
-        <v>88.01000000000001</v>
+        <v>82.73999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1">
-        <v>41</v>
+        <v>147</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8">
-        <v>84.95999999999999</v>
+        <v>80.25</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1">
-        <v>33</v>
+        <v>83</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9">
-        <v>84.72</v>
+        <v>79.20999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10">
-        <v>83.87</v>
+        <v>78.81</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11">
-        <v>81.95</v>
+        <v>78.70999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -732,112 +738,112 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1">
-        <v>137</v>
+        <v>268</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C2">
-        <v>117.69</v>
+        <v>109.25</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1">
-        <v>120</v>
+        <v>143</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C3">
-        <v>112.61</v>
+        <v>102.42</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1">
-        <v>133</v>
+        <v>346</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C4">
-        <v>112.24</v>
+        <v>95.53</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1">
-        <v>21</v>
+        <v>350</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5">
-        <v>102.17</v>
+        <v>92.88</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>177</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6">
-        <v>99.68000000000001</v>
+        <v>92.77</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7">
-        <v>98.78</v>
+        <v>92.44</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1">
-        <v>11</v>
+        <v>368</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8">
-        <v>95.31</v>
+        <v>91.23</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1">
-        <v>77</v>
+        <v>245</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9">
-        <v>91.17</v>
+        <v>90.88</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1">
-        <v>106</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10">
-        <v>90.56</v>
+        <v>90.41</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1">
-        <v>136</v>
+        <v>331</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C11">
-        <v>88.44</v>
+        <v>89.95</v>
       </c>
     </row>
   </sheetData>
@@ -863,112 +869,112 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1">
-        <v>92</v>
+        <v>604</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C2">
-        <v>113.42</v>
+        <v>107.84</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1">
-        <v>211</v>
+        <v>311</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C3">
-        <v>104.08</v>
+        <v>104.81</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1">
-        <v>231</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4">
-        <v>99.84999999999999</v>
+        <v>102.26</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1">
-        <v>37</v>
+        <v>589</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C5">
-        <v>99.39</v>
+        <v>101.5</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
       </c>
       <c r="C6">
-        <v>96.84999999999999</v>
+        <v>100.52</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1">
-        <v>137</v>
+        <v>94</v>
       </c>
       <c r="B7" t="s">
         <v>24</v>
       </c>
       <c r="C7">
-        <v>96.55</v>
+        <v>100.42</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1">
-        <v>192</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
       </c>
       <c r="C8">
-        <v>95.36</v>
+        <v>99.70999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1">
-        <v>190</v>
+        <v>425</v>
       </c>
       <c r="B9" t="s">
         <v>26</v>
       </c>
       <c r="C9">
-        <v>91.62</v>
+        <v>99.22</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="B10" t="s">
         <v>27</v>
       </c>
       <c r="C10">
-        <v>90.45</v>
+        <v>99.18000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1">
-        <v>21</v>
+        <v>260</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C11">
-        <v>89.88</v>
+        <v>98.69</v>
       </c>
     </row>
   </sheetData>
@@ -994,112 +1000,112 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1">
-        <v>266</v>
+        <v>963</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C2">
-        <v>122.26</v>
+        <v>108.75</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1">
-        <v>275</v>
+        <v>378</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3">
-        <v>110.35</v>
+        <v>105.58</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1">
-        <v>182</v>
+        <v>749</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C4">
-        <v>102.57</v>
+        <v>103.81</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1">
-        <v>222</v>
+        <v>938</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C5">
-        <v>97.48</v>
+        <v>103.31</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1">
-        <v>43</v>
+        <v>850</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C6">
-        <v>95.48999999999999</v>
+        <v>103.09</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1">
-        <v>242</v>
+        <v>893</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C7">
-        <v>94.58</v>
+        <v>102.12</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1">
-        <v>280</v>
+        <v>803</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C8">
-        <v>93.05</v>
+        <v>100.28</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1">
-        <v>252</v>
+        <v>628</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C9">
-        <v>92.67</v>
+        <v>99.97</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1">
-        <v>145</v>
+        <v>467</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C10">
-        <v>91.53</v>
+        <v>98.88</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1">
-        <v>221</v>
+        <v>62</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C11">
-        <v>91.51000000000001</v>
+        <v>98.56999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -1125,112 +1131,112 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1">
-        <v>56</v>
+        <v>589</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C2">
-        <v>118.1</v>
+        <v>107.6</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1">
-        <v>16</v>
+        <v>358</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C3">
-        <v>104.49</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C4">
-        <v>99.11</v>
+        <v>103.79</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>582</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C5">
-        <v>98.26000000000001</v>
+        <v>102.78</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1">
-        <v>31</v>
+        <v>278</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="C6">
-        <v>88.37</v>
+        <v>102.26</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1">
-        <v>7</v>
+        <v>439</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C7">
-        <v>86.77</v>
+        <v>101.87</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1">
-        <v>8</v>
+        <v>547</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C8">
-        <v>85.8</v>
+        <v>101.66</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1">
-        <v>15</v>
+        <v>283</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C9">
-        <v>82.93000000000001</v>
+        <v>99.91</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1">
-        <v>25</v>
+        <v>265</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C10">
-        <v>82.53</v>
+        <v>99.76000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1">
-        <v>26</v>
+        <v>250</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C11">
-        <v>81.53</v>
+        <v>99.28</v>
       </c>
     </row>
   </sheetData>
@@ -1256,112 +1262,112 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C2">
-        <v>110.28</v>
+        <v>111.11</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C3">
-        <v>102.95</v>
+        <v>106.42</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1">
-        <v>32</v>
+        <v>274</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C4">
-        <v>87.39</v>
+        <v>104.06</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1">
-        <v>2</v>
+        <v>323</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C5">
-        <v>79.23999999999999</v>
+        <v>103.65</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>179</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C6">
-        <v>78.73999999999999</v>
+        <v>100.47</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1">
-        <v>23</v>
+        <v>307</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C7">
-        <v>77.59999999999999</v>
+        <v>99.65000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C8">
-        <v>74.87</v>
+        <v>98.48</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1">
-        <v>37</v>
+        <v>318</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C9">
-        <v>74.17</v>
+        <v>98.16</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1">
-        <v>31</v>
+        <v>308</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C10">
-        <v>71.66</v>
+        <v>97.86</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1">
-        <v>12</v>
+        <v>376</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C11">
-        <v>70.18000000000001</v>
+        <v>96.73</v>
       </c>
     </row>
   </sheetData>
@@ -1387,112 +1393,112 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C2">
-        <v>97.53</v>
+        <v>107.67</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C3">
-        <v>86.28</v>
+        <v>103.15</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1">
-        <v>26</v>
+        <v>131</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C4">
-        <v>85.2</v>
+        <v>98.31999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="C5">
-        <v>83.73</v>
+        <v>95.56</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="C6">
-        <v>83.51000000000001</v>
+        <v>94.86</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1">
-        <v>54</v>
+        <v>141</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C7">
-        <v>79.48</v>
+        <v>93.34999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C8">
-        <v>77.98999999999999</v>
+        <v>92.94</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C9">
-        <v>73.86</v>
+        <v>89.55</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1">
-        <v>13</v>
+        <v>109</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="C10">
-        <v>73.75</v>
+        <v>89.54000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1">
-        <v>24</v>
+        <v>98</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C11">
-        <v>73.14</v>
+        <v>88.76000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1518,112 +1524,112 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C2">
-        <v>108.24</v>
+        <v>95.89</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C3">
-        <v>77.48999999999999</v>
+        <v>94.33</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C4">
-        <v>75.92</v>
+        <v>92.91</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C5">
-        <v>74.75</v>
+        <v>90.86</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C6">
-        <v>73.01000000000001</v>
+        <v>89.23</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C7">
-        <v>72.45999999999999</v>
+        <v>88.72</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C8">
-        <v>71.41</v>
+        <v>88.47</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C9">
-        <v>67.65000000000001</v>
+        <v>86.48999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C10">
-        <v>66.76000000000001</v>
+        <v>83.95999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C11">
-        <v>66.02</v>
+        <v>82.84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
style: style changes in code
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -7,21 +7,21 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="59" sheetId="1" r:id="rId1"/>
-    <sheet name="66" sheetId="2" r:id="rId2"/>
-    <sheet name="74" sheetId="3" r:id="rId3"/>
-    <sheet name="83" sheetId="4" r:id="rId4"/>
-    <sheet name="93" sheetId="5" r:id="rId5"/>
-    <sheet name="105" sheetId="6" r:id="rId6"/>
-    <sheet name="120" sheetId="7" r:id="rId7"/>
-    <sheet name="120+" sheetId="8" r:id="rId8"/>
+    <sheet name="47" sheetId="1" r:id="rId1"/>
+    <sheet name="52" sheetId="2" r:id="rId2"/>
+    <sheet name="57" sheetId="3" r:id="rId3"/>
+    <sheet name="63" sheetId="4" r:id="rId4"/>
+    <sheet name="69" sheetId="5" r:id="rId5"/>
+    <sheet name="76" sheetId="6" r:id="rId6"/>
+    <sheet name="84" sheetId="7" r:id="rId7"/>
+    <sheet name="84+" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="69">
   <si>
     <t>Name</t>
   </si>
@@ -29,211 +29,205 @@
     <t>Goodlift</t>
   </si>
   <si>
-    <t>Antoine Garcia</t>
-  </si>
-  <si>
-    <t>Etienne Lited</t>
-  </si>
-  <si>
-    <t>Thomas Acher</t>
-  </si>
-  <si>
-    <t>Julien Gutierrez</t>
-  </si>
-  <si>
-    <t>Hermann Charbonnier</t>
-  </si>
-  <si>
-    <t>Thibault Leparc</t>
-  </si>
-  <si>
-    <t>Vincent Todaro</t>
-  </si>
-  <si>
-    <t>Loïz Gautier</t>
-  </si>
-  <si>
-    <t>Gael Pannier</t>
-  </si>
-  <si>
-    <t>Adrien Mailler</t>
-  </si>
-  <si>
-    <t>Panagiotis Tarinidis</t>
-  </si>
-  <si>
-    <t>Hassan El Belghiti</t>
-  </si>
-  <si>
-    <t>Thomas Louet</t>
-  </si>
-  <si>
-    <t>Julien Mercier #2</t>
-  </si>
-  <si>
-    <t>Arthur Hauet</t>
-  </si>
-  <si>
-    <t>Valentin Fruchard</t>
-  </si>
-  <si>
-    <t>Maxime Bataillard</t>
-  </si>
-  <si>
-    <t>Alexandre Tarinidis</t>
-  </si>
-  <si>
-    <t>Steve Vigouroux</t>
-  </si>
-  <si>
-    <t>Paul Rembauville</t>
-  </si>
-  <si>
-    <t>Adrien Poinson</t>
-  </si>
-  <si>
-    <t>Andréa Bonetto</t>
-  </si>
-  <si>
-    <t>Bastien Poyet</t>
-  </si>
-  <si>
-    <t>Alexandre Pont</t>
-  </si>
-  <si>
-    <t>Khaled Benbachir</t>
-  </si>
-  <si>
-    <t>Charly Mairesse</t>
-  </si>
-  <si>
-    <t>Florian Magnier</t>
-  </si>
-  <si>
-    <t>Yanis Bouchou</t>
-  </si>
-  <si>
-    <t>Guillaume Parisot</t>
-  </si>
-  <si>
-    <t>Pierre Renaud</t>
-  </si>
-  <si>
-    <t>Valentin Cure</t>
-  </si>
-  <si>
-    <t>Souleiman Turki</t>
-  </si>
-  <si>
-    <t>Thomas Czaplicki</t>
-  </si>
-  <si>
-    <t>Romain Picot-Guéraud</t>
-  </si>
-  <si>
-    <t>Maxime Girard</t>
-  </si>
-  <si>
-    <t>Joris Quai</t>
-  </si>
-  <si>
-    <t>Anthony Costarigot</t>
-  </si>
-  <si>
-    <t>Richmond Baiden</t>
-  </si>
-  <si>
-    <t>Julien Balangwe Bakinien</t>
-  </si>
-  <si>
-    <t>Ali Ben Hadj Ali</t>
-  </si>
-  <si>
-    <t>Quentin Gilbert</t>
-  </si>
-  <si>
-    <t>Guillaume Jean Marie Flore</t>
-  </si>
-  <si>
-    <t>Malik Bernoussi Triolet</t>
-  </si>
-  <si>
-    <t>Paco Castillo</t>
-  </si>
-  <si>
-    <t>Gil Pinheiro</t>
-  </si>
-  <si>
-    <t>Gabriel Begue</t>
-  </si>
-  <si>
-    <t>Corentin Clément</t>
-  </si>
-  <si>
-    <t>Nicolas Peyraud</t>
-  </si>
-  <si>
-    <t>Sofiane Belkesir</t>
-  </si>
-  <si>
-    <t>Benoit Carole</t>
-  </si>
-  <si>
-    <t>Sami Maury</t>
-  </si>
-  <si>
-    <t>Rekendy Faufil</t>
-  </si>
-  <si>
-    <t>Youssuf El Adlani</t>
-  </si>
-  <si>
-    <t>Antoine De Rohden</t>
-  </si>
-  <si>
-    <t>Charly Boucher</t>
-  </si>
-  <si>
-    <t>Tony Bayrakcioglu</t>
-  </si>
-  <si>
-    <t>Frédéric Lecellier</t>
-  </si>
-  <si>
-    <t>Andy Richon</t>
-  </si>
-  <si>
-    <t>Nour-Eddine Ghaoui</t>
-  </si>
-  <si>
-    <t>Marcus Feliho</t>
-  </si>
-  <si>
-    <t>Romuald Massé</t>
-  </si>
-  <si>
-    <t>Stanley Odin</t>
-  </si>
-  <si>
-    <t>Julien Moala</t>
-  </si>
-  <si>
-    <t>Ugo Masarotti</t>
-  </si>
-  <si>
-    <t>Paulin Mbakop Kweffo</t>
-  </si>
-  <si>
-    <t>Abdellah Hassar</t>
-  </si>
-  <si>
-    <t>Karim Messai</t>
-  </si>
-  <si>
-    <t>Éric Bonin</t>
-  </si>
-  <si>
-    <t>Abdelaziz Benikken</t>
+    <t>Tiffany Chapon</t>
+  </si>
+  <si>
+    <t>Noémie Allabert</t>
+  </si>
+  <si>
+    <t>Stéphanie Legard</t>
+  </si>
+  <si>
+    <t>Andréa Zicaro</t>
+  </si>
+  <si>
+    <t>Bénédicte LePanse</t>
+  </si>
+  <si>
+    <t>Cathy Phatien</t>
+  </si>
+  <si>
+    <t>Nathalie Piantino</t>
+  </si>
+  <si>
+    <t>Marianne Bouvard</t>
+  </si>
+  <si>
+    <t>Yvelise Martin</t>
+  </si>
+  <si>
+    <t>Nathalie Feraud</t>
+  </si>
+  <si>
+    <t>Shizuka Rico</t>
+  </si>
+  <si>
+    <t>Camille Hadrys</t>
+  </si>
+  <si>
+    <t>Alison Huet</t>
+  </si>
+  <si>
+    <t>Laurie Julien</t>
+  </si>
+  <si>
+    <t>Anna Maramotti</t>
+  </si>
+  <si>
+    <t>Lorraine Balbiani</t>
+  </si>
+  <si>
+    <t>Maëva Lambert</t>
+  </si>
+  <si>
+    <t>Jade Jacob</t>
+  </si>
+  <si>
+    <t>Océane Regis</t>
+  </si>
+  <si>
+    <t>Sovannphaktra Pal</t>
+  </si>
+  <si>
+    <t>Caroline Suné</t>
+  </si>
+  <si>
+    <t>Agnès Alves</t>
+  </si>
+  <si>
+    <t>Léa Gratacos</t>
+  </si>
+  <si>
+    <t>Mélodie Anthouard</t>
+  </si>
+  <si>
+    <t>Mélanie Pagesy</t>
+  </si>
+  <si>
+    <t>Marina Soyer-Bardi</t>
+  </si>
+  <si>
+    <t>Prescillia Bavoil</t>
+  </si>
+  <si>
+    <t>Samantha Eugenie</t>
+  </si>
+  <si>
+    <t>Ludivine Delos</t>
+  </si>
+  <si>
+    <t>Mathilde Rosset</t>
+  </si>
+  <si>
+    <t>Sarah Saint Aime</t>
+  </si>
+  <si>
+    <t>Justine Jouve</t>
+  </si>
+  <si>
+    <t>Mathilde Pataille</t>
+  </si>
+  <si>
+    <t>Clara Peyraud</t>
+  </si>
+  <si>
+    <t>Pauline Le Bras</t>
+  </si>
+  <si>
+    <t>Andorina Bouchoux</t>
+  </si>
+  <si>
+    <t>Bertille Hedon</t>
+  </si>
+  <si>
+    <t>Camille Pailha</t>
+  </si>
+  <si>
+    <t>Clara Kaminski</t>
+  </si>
+  <si>
+    <t>Haingotiana Rasamimanantsoa</t>
+  </si>
+  <si>
+    <t>Isoline Berger</t>
+  </si>
+  <si>
+    <t>Laura Mautalen</t>
+  </si>
+  <si>
+    <t>Margot Concolato</t>
+  </si>
+  <si>
+    <t>Angeline Berva</t>
+  </si>
+  <si>
+    <t>Christelle Mouandjo</t>
+  </si>
+  <si>
+    <t>Jessica Doorhyee</t>
+  </si>
+  <si>
+    <t>France Juilien</t>
+  </si>
+  <si>
+    <t>Pauline Leroux</t>
+  </si>
+  <si>
+    <t>Ludivine Leroy</t>
+  </si>
+  <si>
+    <t>Elisa Elleuch</t>
+  </si>
+  <si>
+    <t>Kelly Millecamps</t>
+  </si>
+  <si>
+    <t>Lea Schreiner</t>
+  </si>
+  <si>
+    <t>Innès Allouache</t>
+  </si>
+  <si>
+    <t>Marion Attelly</t>
+  </si>
+  <si>
+    <t>Julie Franch Guerra</t>
+  </si>
+  <si>
+    <t>Cécile Brotons</t>
+  </si>
+  <si>
+    <t>France Collinot</t>
+  </si>
+  <si>
+    <t>Amélie Mierger</t>
+  </si>
+  <si>
+    <t>Marie Stéphanie Vili</t>
+  </si>
+  <si>
+    <t>Rachelle Letaief</t>
+  </si>
+  <si>
+    <t>Atonina Vehikite</t>
+  </si>
+  <si>
+    <t>Cindy Hebe</t>
+  </si>
+  <si>
+    <t>Camille Dezier</t>
+  </si>
+  <si>
+    <t>Albane Benitah</t>
+  </si>
+  <si>
+    <t>Jennifer Bailleul</t>
+  </si>
+  <si>
+    <t>Camellia Messaoui</t>
+  </si>
+  <si>
+    <t>Angélique Lafont</t>
   </si>
 </sst>
 </file>
@@ -607,13 +601,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2">
-        <v>94.15000000000001</v>
+        <v>118.48</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -624,95 +618,95 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>93.94</v>
+        <v>104.62</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1">
-        <v>137</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4">
-        <v>90.45</v>
+        <v>101.62</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1">
-        <v>75</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5">
-        <v>89.2</v>
+        <v>92.38</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6">
-        <v>84.81999999999999</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7">
-        <v>82.73999999999999</v>
+        <v>88.01000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1">
-        <v>147</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8">
-        <v>80.25</v>
+        <v>84.95999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1">
-        <v>83</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9">
-        <v>79.20999999999999</v>
+        <v>84.72</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10">
-        <v>78.81</v>
+        <v>83.87</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11">
-        <v>78.70999999999999</v>
+        <v>81.95</v>
       </c>
     </row>
   </sheetData>
@@ -738,112 +732,112 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1">
-        <v>268</v>
+        <v>137</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>109.25</v>
+        <v>117.69</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>102.42</v>
+        <v>112.61</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1">
-        <v>346</v>
+        <v>133</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C4">
-        <v>95.53</v>
+        <v>112.24</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1">
-        <v>350</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5">
-        <v>92.88</v>
+        <v>102.17</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1">
-        <v>177</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6">
-        <v>92.77</v>
+        <v>99.68000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7">
-        <v>92.44</v>
+        <v>98.78</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1">
-        <v>368</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8">
-        <v>91.23</v>
+        <v>95.31</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1">
-        <v>245</v>
+        <v>77</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9">
-        <v>90.88</v>
+        <v>91.17</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1">
-        <v>19</v>
+        <v>106</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10">
-        <v>90.41</v>
+        <v>90.56</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1">
-        <v>331</v>
+        <v>136</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C11">
-        <v>89.95</v>
+        <v>88.44</v>
       </c>
     </row>
   </sheetData>
@@ -869,112 +863,112 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1">
-        <v>604</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C2">
-        <v>107.84</v>
+        <v>113.42</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1">
-        <v>311</v>
+        <v>211</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C3">
-        <v>104.81</v>
+        <v>104.08</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1">
-        <v>7</v>
+        <v>231</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4">
-        <v>102.26</v>
+        <v>99.84999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1">
-        <v>589</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C5">
-        <v>101.5</v>
+        <v>99.39</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1">
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
       </c>
       <c r="C6">
-        <v>100.52</v>
+        <v>96.84999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1">
-        <v>94</v>
+        <v>137</v>
       </c>
       <c r="B7" t="s">
         <v>24</v>
       </c>
       <c r="C7">
-        <v>100.42</v>
+        <v>96.55</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1">
-        <v>20</v>
+        <v>192</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
       </c>
       <c r="C8">
-        <v>99.70999999999999</v>
+        <v>95.36</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1">
-        <v>425</v>
+        <v>190</v>
       </c>
       <c r="B9" t="s">
         <v>26</v>
       </c>
       <c r="C9">
-        <v>99.22</v>
+        <v>91.62</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="B10" t="s">
         <v>27</v>
       </c>
       <c r="C10">
-        <v>99.18000000000001</v>
+        <v>90.45</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1">
-        <v>260</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C11">
-        <v>98.69</v>
+        <v>89.88</v>
       </c>
     </row>
   </sheetData>
@@ -1000,112 +994,112 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1">
-        <v>963</v>
+        <v>266</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2">
-        <v>108.75</v>
+        <v>122.26</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1">
-        <v>378</v>
+        <v>275</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3">
-        <v>105.58</v>
+        <v>110.35</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1">
-        <v>749</v>
+        <v>182</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4">
-        <v>103.81</v>
+        <v>102.57</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1">
-        <v>938</v>
+        <v>222</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5">
-        <v>103.31</v>
+        <v>97.48</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1">
-        <v>850</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C6">
-        <v>103.09</v>
+        <v>95.48999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1">
-        <v>893</v>
+        <v>242</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C7">
-        <v>102.12</v>
+        <v>94.58</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1">
-        <v>803</v>
+        <v>280</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C8">
-        <v>100.28</v>
+        <v>93.05</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1">
-        <v>628</v>
+        <v>252</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="C9">
-        <v>99.97</v>
+        <v>92.67</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1">
-        <v>467</v>
+        <v>145</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C10">
-        <v>98.88</v>
+        <v>91.53</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1">
-        <v>62</v>
+        <v>221</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C11">
-        <v>98.56999999999999</v>
+        <v>91.51000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1131,112 +1125,112 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1">
-        <v>589</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C2">
-        <v>107.6</v>
+        <v>118.1</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1">
-        <v>358</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C3">
-        <v>105</v>
+        <v>104.49</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C4">
-        <v>103.79</v>
+        <v>99.11</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1">
-        <v>582</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C5">
-        <v>102.78</v>
+        <v>98.26000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1">
-        <v>278</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C6">
-        <v>102.26</v>
+        <v>88.37</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1">
-        <v>439</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C7">
-        <v>101.87</v>
+        <v>86.77</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1">
-        <v>547</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C8">
-        <v>101.66</v>
+        <v>85.8</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1">
-        <v>283</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C9">
-        <v>99.91</v>
+        <v>82.93000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1">
-        <v>265</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C10">
-        <v>99.76000000000001</v>
+        <v>82.53</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1">
-        <v>250</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C11">
-        <v>99.28</v>
+        <v>81.53</v>
       </c>
     </row>
   </sheetData>
@@ -1262,112 +1256,112 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C2">
-        <v>111.11</v>
+        <v>110.28</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C3">
-        <v>106.42</v>
+        <v>102.95</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1">
-        <v>274</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C4">
-        <v>104.06</v>
+        <v>87.39</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1">
-        <v>323</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C5">
-        <v>103.65</v>
+        <v>79.23999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1">
-        <v>179</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C6">
-        <v>100.47</v>
+        <v>78.73999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1">
-        <v>307</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C7">
-        <v>99.65000000000001</v>
+        <v>77.59999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C8">
-        <v>98.48</v>
+        <v>74.87</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1">
-        <v>318</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C9">
-        <v>98.16</v>
+        <v>74.17</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1">
-        <v>308</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C10">
-        <v>97.86</v>
+        <v>71.66</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1">
-        <v>376</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C11">
-        <v>96.73</v>
+        <v>70.18000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1393,112 +1387,112 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1">
-        <v>107</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C2">
-        <v>107.67</v>
+        <v>97.53</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C3">
-        <v>103.15</v>
+        <v>86.28</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1">
-        <v>131</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C4">
-        <v>98.31999999999999</v>
+        <v>85.2</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="C5">
-        <v>95.56</v>
+        <v>83.73</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C6">
-        <v>94.86</v>
+        <v>83.51000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1">
-        <v>141</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C7">
-        <v>93.34999999999999</v>
+        <v>79.48</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C8">
-        <v>92.94</v>
+        <v>77.98999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C9">
-        <v>89.55</v>
+        <v>73.86</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1">
-        <v>109</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="C10">
-        <v>89.54000000000001</v>
+        <v>73.75</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C11">
-        <v>88.76000000000001</v>
+        <v>73.14</v>
       </c>
     </row>
   </sheetData>
@@ -1524,112 +1518,112 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1">
-        <v>51</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C2">
-        <v>95.89</v>
+        <v>108.24</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C3">
-        <v>94.33</v>
+        <v>77.48999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C4">
-        <v>92.91</v>
+        <v>75.92</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1">
-        <v>59</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C5">
-        <v>90.86</v>
+        <v>74.75</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C6">
-        <v>89.23</v>
+        <v>73.01000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C7">
-        <v>88.72</v>
+        <v>72.45999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C8">
-        <v>88.47</v>
+        <v>71.41</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C9">
-        <v>86.48999999999999</v>
+        <v>67.65000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1">
-        <v>64</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C10">
-        <v>83.95999999999999</v>
+        <v>66.76000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C11">
-        <v>82.84</v>
+        <v>66.02</v>
       </c>
     </row>
   </sheetData>

</xml_diff>